<commit_message>
the excel way done
</commit_message>
<xml_diff>
--- a/week-7-alternatives-python/video7-small_movies.xlsx
+++ b/week-7-alternatives-python/video7-small_movies.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27224"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelsjoberg/Dropbox/- STUDIES/edX/DelftX/EX101x Data Analysis Take it to the MAX()/week-7-alternatives-python/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="100" windowWidth="17300" windowHeight="11700" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="14120" yWindow="4160" windowWidth="14860" windowHeight="11700" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="_ironspread_data_" sheetId="4" state="veryHidden" r:id="rId1"/>
@@ -14,6 +19,9 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -22,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
   <si>
     <t>Kevin Bacon</t>
   </si>
@@ -79,6 +87,21 @@
   </si>
   <si>
     <t>C:\Users\Felienne\Dropbox\TU Delft\Courses\MOOC\Examples\Movie\BaconMin.py</t>
+  </si>
+  <si>
+    <t>Is this Bacon?</t>
+  </si>
+  <si>
+    <t>Steps to Movie 1</t>
+  </si>
+  <si>
+    <t>Step 1</t>
+  </si>
+  <si>
+    <t>Steps from Movie 1</t>
+  </si>
+  <si>
+    <t>Step 2</t>
   </si>
 </sst>
 </file>
@@ -185,12 +208,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -220,12 +243,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -433,14 +456,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -448,7 +471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -456,7 +479,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -466,243 +489,402 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <f>SUMIF(Movie_Actor!$B$1:$B$12,A2,Movie_Actor!$C$1:$C$12)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <f>SUMIF(Movie_Actor!$B$1:$B$12,A3,Movie_Actor!$C$1:$C$12)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <f>SUMIF(Movie_Actor!$B$1:$B$12,A4,Movie_Actor!$C$1:$C$12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
+      </c>
+      <c r="B5">
+        <f>SUMIF(Movie_Actor!$B$1:$B$12,A5,Movie_Actor!$C$1:$C$12)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <f>IF(A2="Kevin Bacon",1,"-")</f>
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>IFERROR(MIN(B2,VLOOKUP(A2,Movie_Actor!$A$1:$D$12,4,FALSE)),"-")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B8" si="0">IF(A3="Kevin Bacon",1,"-")</f>
+        <v>-</v>
+      </c>
+      <c r="C3">
+        <f>IFERROR(MIN(B3,VLOOKUP(A3,Movie_Actor!$A$1:$D$12,4,FALSE)),"-")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="C4">
+        <f>IFERROR(MIN(B4,VLOOKUP(A4,Movie_Actor!$A$1:$D$12,4,FALSE)),"-")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="C5">
+        <f>IFERROR(MIN(B5,VLOOKUP(A5,Movie_Actor!$A$1:$D$12,4,FALSE)),"-")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="C6">
+        <f>IFERROR(MIN(B6,VLOOKUP(A6,Movie_Actor!$A$1:$D$12,4,FALSE)),"-")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="C7" t="str">
+        <f>IFERROR(MIN(B7,VLOOKUP(A7,Movie_Actor!$A$1:$D$12,4,FALSE)),"-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="C8" t="str">
+        <f>IFERROR(MIN(B8,VLOOKUP(A8,Movie_Actor!$A$1:$D$12,4,FALSE)),"-")</f>
+        <v>-</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <f>VLOOKUP(A2,Actor!$A$1:$B$8,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>IF(VLOOKUP(B2,Movie!$A$1:$B$5,2,FALSE)=0,"-",VLOOKUP(B2,Movie!$A$1:$B$5,2,FALSE)+1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" t="str">
+        <f>VLOOKUP(A3,Actor!$A$1:$B$8,2,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="D3">
+        <f>IF(VLOOKUP(B3,Movie!$A$1:$B$5,2,FALSE)=0,"-",VLOOKUP(B3,Movie!$A$1:$B$5,2,FALSE)+1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" t="str">
+        <f>VLOOKUP(A4,Actor!$A$1:$B$8,2,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="D4">
+        <f>IF(VLOOKUP(B4,Movie!$A$1:$B$5,2,FALSE)=0,"-",VLOOKUP(B4,Movie!$A$1:$B$5,2,FALSE)+1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" t="str">
+        <f>VLOOKUP(A5,Actor!$A$1:$B$8,2,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="D5">
+        <f>IF(VLOOKUP(B5,Movie!$A$1:$B$5,2,FALSE)=0,"-",VLOOKUP(B5,Movie!$A$1:$B$5,2,FALSE)+1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <f>VLOOKUP(A6,Actor!$A$1:$B$8,2,FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <f>IF(VLOOKUP(B6,Movie!$A$1:$B$5,2,FALSE)=0,"-",VLOOKUP(B6,Movie!$A$1:$B$5,2,FALSE)+1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" t="str">
+        <f>VLOOKUP(A7,Actor!$A$1:$B$8,2,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="D7">
+        <f>IF(VLOOKUP(B7,Movie!$A$1:$B$5,2,FALSE)=0,"-",VLOOKUP(B7,Movie!$A$1:$B$5,2,FALSE)+1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" t="str">
+        <f>VLOOKUP(A8,Actor!$A$1:$B$8,2,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="D8" t="str">
+        <f>IF(VLOOKUP(B8,Movie!$A$1:$B$5,2,FALSE)=0,"-",VLOOKUP(B8,Movie!$A$1:$B$5,2,FALSE)+1)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" t="str">
+        <f>VLOOKUP(A9,Actor!$A$1:$B$8,2,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="D9" t="str">
+        <f>IF(VLOOKUP(B9,Movie!$A$1:$B$5,2,FALSE)=0,"-",VLOOKUP(B9,Movie!$A$1:$B$5,2,FALSE)+1)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" t="str">
+        <f>VLOOKUP(A10,Actor!$A$1:$B$8,2,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="D10" t="str">
+        <f>IF(VLOOKUP(B10,Movie!$A$1:$B$5,2,FALSE)=0,"-",VLOOKUP(B10,Movie!$A$1:$B$5,2,FALSE)+1)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C11" t="str">
+        <f>VLOOKUP(A11,Actor!$A$1:$B$8,2,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="D11" t="str">
+        <f>IF(VLOOKUP(B11,Movie!$A$1:$B$5,2,FALSE)=0,"-",VLOOKUP(B11,Movie!$A$1:$B$5,2,FALSE)+1)</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
+      <c r="C12" t="str">
+        <f>VLOOKUP(A12,Actor!$A$1:$B$8,2,FALSE)</f>
+        <v>-</v>
+      </c>
+      <c r="D12" t="str">
+        <f>IF(VLOOKUP(B12,Movie!$A$1:$B$5,2,FALSE)=0,"-",VLOOKUP(B12,Movie!$A$1:$B$5,2,FALSE)+1)</f>
+        <v>-</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>